<commit_message>
fix import siswa dan guru
</commit_message>
<xml_diff>
--- a/upload/format_import_pengajar.xlsx
+++ b/upload/format_import_pengajar.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">sengklek123</t>
   </si>
   <si>
-    <t xml:space="preserve">Dikreg999 </t>
+    <t xml:space="preserve">Matematika, Bahasa Indonesia </t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -188,7 +188,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1012" min="12" style="0" width="8.76"/>

</xml_diff>